<commit_message>
updated examples and usage
</commit_message>
<xml_diff>
--- a/examples/configuration_workbook/files/data.xlsx
+++ b/examples/configuration_workbook/files/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariel/Documents/repos/go/src/terraform-provider-config/examples/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\go\src\terraform-provider-config\examples\configuration_workbook\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709203C7-634B-F647-A5D7-F73A6E1F547C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129D551-90BB-42F7-B208-F0F04E26F4B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12700" yWindow="4600" windowWidth="19200" windowHeight="12080" activeTab="1" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
+    <workbookView xWindow="12700" yWindow="4600" windowWidth="19200" windowHeight="12080" activeTab="2" xr2:uid="{B0AD3E86-2D5D-41DA-902C-D5987C5C163C}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="Vert" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -497,12 +498,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -572,7 +573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -601,7 +602,7 @@
         <v>4.1550000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -631,13 +632,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86D689-62A5-2C4B-BADF-72219E6A3529}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -645,7 +646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -653,7 +654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -664,5 +665,19 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B1037F-BDEC-4ACA-BF04-E80D13CF3D41}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>